<commit_message>
Upload updated versions of the light trap files
</commit_message>
<xml_diff>
--- a/larval_size_analysis/Means_Table.xlsx
+++ b/larval_size_analysis/Means_Table.xlsx
@@ -411,10 +411,10 @@
         <v>6</v>
       </c>
       <c r="C4" t="n">
-        <v>6.03253012048193</v>
+        <v>5.97371428571429</v>
       </c>
       <c r="D4" t="n">
-        <v>166</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5">
@@ -425,10 +425,10 @@
         <v>7</v>
       </c>
       <c r="C5" t="n">
-        <v>5.19917355371901</v>
+        <v>5.19856</v>
       </c>
       <c r="D5" t="n">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6">
@@ -481,10 +481,10 @@
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>2.81163895486936</v>
+        <v>2.77320430107527</v>
       </c>
       <c r="D9" t="n">
-        <v>421</v>
+        <v>465</v>
       </c>
     </row>
     <row r="10">
@@ -495,10 +495,10 @@
         <v>7</v>
       </c>
       <c r="C10" t="n">
-        <v>2.41530612244898</v>
+        <v>2.42452153110048</v>
       </c>
       <c r="D10" t="n">
-        <v>393</v>
+        <v>419</v>
       </c>
     </row>
     <row r="11">
@@ -509,10 +509,10 @@
         <v>8</v>
       </c>
       <c r="C11" t="n">
-        <v>2.55882352941176</v>
+        <v>2.54321428571429</v>
       </c>
       <c r="D11" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>